<commit_message>
change list of audios
</commit_message>
<xml_diff>
--- a/audio-train.xlsx
+++ b/audio-train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FAKS\_DUBOKO_UCENJE\Sentiment-Analysis-Voice-Recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312843D0-BDEC-4E4C-8C4A-8F1136018609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0DA8DE-8012-4497-8569-1A3683572DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,42 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>file</t>
   </si>
   <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>/audio/female1.wav</t>
-  </si>
-  <si>
-    <t>analyze sentiment of</t>
-  </si>
-  <si>
-    <t>/audio/female2.wav</t>
-  </si>
-  <si>
-    <t>/audio/female5.wav</t>
-  </si>
-  <si>
-    <t>/audio/female7.wav</t>
-  </si>
-  <si>
-    <t>/audio/male1.wav</t>
-  </si>
-  <si>
-    <t>/audio/male2.wav</t>
-  </si>
-  <si>
-    <t>/audio/female8.wav</t>
-  </si>
-  <si>
-    <t>/audio/female4.wav</t>
-  </si>
-  <si>
-    <t>/audio/female9.wav</t>
   </si>
   <si>
     <t>/audio/sentence1.wav</t>
@@ -522,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,23 +517,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -571,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -579,255 +549,183 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>